<commit_message>
amélioration design en repsonsive portrait et gestion du theme par cookie js
</commit_message>
<xml_diff>
--- a/assets/data/data.xlsx
+++ b/assets/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dim\clone_repo\portfolio\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B8BF94-03F3-40E6-A49E-4270AC88D217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9528151-B1CE-46E6-8FDA-9462C8E6BC23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
   <si>
     <t>title</t>
   </si>
@@ -275,6 +275,27 @@
   </si>
   <si>
     <t>judo_tracking.webm</t>
+  </si>
+  <si>
+    <t>img_results</t>
+  </si>
+  <si>
+    <t>alt_img_results</t>
+  </si>
+  <si>
+    <t>illustration résultats Analyse IA Judo</t>
+  </si>
+  <si>
+    <t>url_img_data</t>
+  </si>
+  <si>
+    <t>alt_img_data</t>
+  </si>
+  <si>
+    <t>AI_Judo_data.webp</t>
+  </si>
+  <si>
+    <t>AI_Judo_results.webp</t>
   </si>
 </sst>
 </file>
@@ -351,7 +372,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -662,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V25"/>
+  <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,18 +703,19 @@
     <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.28515625" customWidth="1"/>
-    <col min="17" max="17" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="165.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="47.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="32.7109375" customWidth="1"/>
+    <col min="14" max="15" width="17.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="24.28515625" customWidth="1"/>
+    <col min="21" max="21" width="165.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="32.7109375" customWidth="1"/>
+    <col min="25" max="25" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>80</v>
       </c>
@@ -734,34 +756,46 @@
         <v>66</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -780,11 +814,11 @@
       <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -803,11 +837,11 @@
       <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="S3" t="s">
+      <c r="U3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -826,14 +860,14 @@
       <c r="F4" t="s">
         <v>21</v>
       </c>
-      <c r="S4" t="s">
+      <c r="U4" t="s">
         <v>19</v>
       </c>
-      <c r="T4" t="s">
+      <c r="V4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -852,14 +886,14 @@
       <c r="F5" t="s">
         <v>26</v>
       </c>
-      <c r="S5" t="s">
+      <c r="U5" t="s">
         <v>24</v>
       </c>
-      <c r="T5" t="s">
+      <c r="V5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -896,26 +930,38 @@
       <c r="L6" t="s">
         <v>78</v>
       </c>
+      <c r="N6" t="s">
+        <v>90</v>
+      </c>
       <c r="O6" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q6" t="s">
         <v>79</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="R6" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="S6" t="s">
+        <v>91</v>
+      </c>
+      <c r="T6" t="s">
+        <v>87</v>
+      </c>
+      <c r="V6" t="s">
+        <v>29</v>
+      </c>
+      <c r="X6" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y6" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="R6" s="3" t="s">
+      <c r="Z6" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="T6" t="s">
-        <v>29</v>
-      </c>
-      <c r="V6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -934,11 +980,11 @@
       <c r="F7" t="s">
         <v>35</v>
       </c>
-      <c r="T7" t="s">
+      <c r="V7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -957,14 +1003,14 @@
       <c r="F8" t="s">
         <v>41</v>
       </c>
-      <c r="T8" t="s">
+      <c r="V8" t="s">
         <v>39</v>
       </c>
-      <c r="U8" t="s">
+      <c r="W8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -983,11 +1029,11 @@
       <c r="F9" t="s">
         <v>46</v>
       </c>
-      <c r="T9" t="s">
+      <c r="V9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1006,18 +1052,18 @@
       <c r="F10" t="s">
         <v>50</v>
       </c>
-      <c r="T10" t="s">
+      <c r="V10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O23" s="4"/>
-    </row>
-    <row r="24" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O24" s="4"/>
-    </row>
-    <row r="25" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O25" s="4"/>
+    <row r="23" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q23" s="4"/>
+    </row>
+    <row r="24" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q24" s="4"/>
+    </row>
+    <row r="25" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q25" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
modification css pour fiche projet lanscape
</commit_message>
<xml_diff>
--- a/assets/data/data.xlsx
+++ b/assets/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dim\clone_repo\portfolio\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9528151-B1CE-46E6-8FDA-9462C8E6BC23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A183776F-62ED-499A-A8F2-0991E7AB6CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="202">
   <si>
     <t>title</t>
   </si>
@@ -296,13 +296,514 @@
   </si>
   <si>
     <t>AI_Judo_results.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plusieurs millions de lignes (Collectées toutes les minutes pendant plusieurs années </t>
+  </si>
+  <si>
+    <t>Données temporelles quantitatives (quantités produites, durées des arrêts, cadences) et qualitatives (état des équipements, anomalies, dysfonctionnements).</t>
+  </si>
+  <si>
+    <t>Les données intègrent des anomalies et des irrégularités temporelles, avec potentiellement des périodes d'absence ou des états incohérents des machines.</t>
+  </si>
+  <si>
+    <t>Power BI (visualisation, rapport)
+|-|
+DAX (calculs avancés, KPIs)
+|-|
+Python (prétraitement, analyse exploratoire)
+|-|
+Microsoft SQL Server (gestion de données)</t>
+  </si>
+  <si>
+    <t>Nécessité d'améliorer la mesure de la productivité, d'identifier les causes d’arrêts machine fréquents, et d'optimiser la gestion des formats de conditionnement.</t>
+  </si>
+  <si>
+    <t>Analyser la performance opérationnelle pour définir un plan d'amélioration qui permette de gagner en productivité</t>
+  </si>
+  <si>
+    <t>Projet industriel visant à optimiser la productivité d'un atelier de conditionnement de peinture en surveillant performances, cadences et temps d'arrêts détaillés. L'objectif était également d'obtenir une meilleure visibilité sur les quantités conditionnées selon les formats spécifiques utilisés, afin de faciliter la prise de décision opérationnelle et stratégique. Ce projet nécessitait l'exploitation approfondie de données opérationnelles collectées en continu, permettant d’identifier clairement les problématiques récurrentes et d’améliorer le rendement global des lignes de conditionnement.</t>
+  </si>
+  <si>
+    <t>Base Microsoft SQL Serve (données confidentielles)</t>
+  </si>
+  <si>
+    <t>Rapport Power BI permettant une visualisation claire des performances de la ligne.
+|-|
+Analyse détaillée des impacts des arrêts programmés et non programmés sur la cadence.
+|-|
+La mise en place de ces rapports a permis d'élaborer des plans d'action qui ont réduit les dysfonctionnements techniques de 10 à 15%.
+|-|
+Amélioration globale de la performance avec une augmentation de 10% du TRS.</t>
+  </si>
+  <si>
+    <t>Illustration rapport power BI</t>
+  </si>
+  <si>
+    <t>pwBI_pilotage_atelier.webp</t>
+  </si>
+  <si>
+    <t>pwBI_pilotage_atelier_data.webp</t>
+  </si>
+  <si>
+    <t>Difficultés rencontrées dans l'intégration et le nettoyage des données en raison de la quantité de données à traiter.
+|-|
+Nécessité de sensibiliser les équipes terrain à l'importance de la saisie et des déclarations régulières et précise des données.</t>
+  </si>
+  <si>
+    <t>Mise en place de systèmes d'alerte proactive pour anticiper les dysfonctionnements potentiels.
+|-|
+Développement d'une interface utilisateur améliorée facilitant l'exploitation des rapports par les équipes opérationnelles.</t>
+  </si>
+  <si>
+    <t>Projet basé sur l'analyse d'un jeu de données public issu de Kaggle relatif aux trajets des taxis de New York. L'objectif principal était d’explorer les données disponibles pour détecter des tendances en matière de déplacements urbains, identifier des anomalies potentielles et améliorer les décisions stratégiques d’affectation des ressources.</t>
+  </si>
+  <si>
+    <t>Effectuer un traitement approfondi pour nettoyer, structurer et analyser les données afin d'optimiser la répartition des taxis, leur rentabilité et l'efficacité opérationnelle.</t>
+  </si>
+  <si>
+    <t>Nécessité d'améliorer la disponibilité des taxis, la rentabilité des trajets et l’efficacité opérationnelle grâce à une meilleure compréhension des comportements des utilisateurs et des anomalies éventuelles.</t>
+  </si>
+  <si>
+    <t>NYC Taxi Trips Dataset issu de Kaggle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grande volumétrie, plus de 30 millions de lignes </t>
+  </si>
+  <si>
+    <t>Données temporelles et géospatiales, quantitatives (durée, distance, tarifs) et qualitatives (états du véhicule, types de paiement, localisation)</t>
+  </si>
+  <si>
+    <t>Présence importante de valeurs aberrantes nécessitant une gestion minutieuse pour assurer la qualité et la pertinence des analyses</t>
+  </si>
+  <si>
+    <t>Gestion complexe des anomalies dues aux données volumineuses et hétérogènes.
+|-|
+Nécessité de maîtriser les techniques avancées de nettoyage et structuration de données géospatiales.
+|-|
+Apprentissage approfondi de l'intégration efficace de Python et SQL pour la gestion de grands volumes de données.</t>
+  </si>
+  <si>
+    <t>Mise en évidence des principales tendances des trajets.
+|-|
+Identification claire et gestion efficace des anomalies.
+|-|
+Optimisation significative du stockage et de l’accès rapide aux données.</t>
+  </si>
+  <si>
+    <t>Extraction et téléchargement des données depuis Kaggle.
+|-|
+Conversion des données en format Parquet pour optimisation du stockage.
+|-|
+Nettoyage et structuration des données avec Python.
+|-|
+Identification et gestion des valeurs aberrantes.
+|-|
+Traitement avancé des données avec PostgreSQL.
+|-|
+Visualisation interactive des données avec Power BI.</t>
+  </si>
+  <si>
+    <t>Automatisation accrue du processus complet d'intégration et d'analyse pour permettre des mises à jour régulières.</t>
+  </si>
+  <si>
+    <t>Python (Pandas, NumPy, Geopandas, geoalchemy2, sqlalchemy, statsmodels)
+|-|
+Jupyter Notebook
+|-|
+PostgreSQL (optimisation et agrégation de données)
+|-|
+Power BI (visualisations interactives)</t>
+  </si>
+  <si>
+    <t>pwBI_taxi_results.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Illustration résultat visualisation power BI </t>
+  </si>
+  <si>
+    <t>pwBI_taxi_data.webp</t>
+  </si>
+  <si>
+    <t>Illustration des data en shéma étoile</t>
+  </si>
+  <si>
+    <t>pwBI_data20_results.webp</t>
+  </si>
+  <si>
+    <t>Le Domaine des Croix, un vignoble bourguignon, souhaite s’implanter sur le marché américain. Ce projet vise à étudier les tendances du marché, évaluer la compétitivité des vins, notamment les Pinot Noir de Bourgogne, et à recommander une stratégie tarifaire adaptée pour valoriser la qualité de leurs produits tout en restant compétitif.</t>
+  </si>
+  <si>
+    <t>130 000 entrées environ</t>
+  </si>
+  <si>
+    <t>Jeu de données publiques et Fiche descriptive spécifique du vin du Domaine des Croix</t>
+  </si>
+  <si>
+    <t>Données quantitatives (prix, notes des œnologues) et qualitatives (cépages, régions de production, descriptifs).</t>
+  </si>
+  <si>
+    <t>Nécessité d'un nettoyage rigoureux en raison des valeurs manquantes ou aberrantes, uniformisation des données en termes de devises et de millésimes.</t>
+  </si>
+  <si>
+    <t>Utilisation de modèles prédictifs pour anticiper les évolutions futures du marché.
+|-|
+Enrichissement des données avec des sources externes pour affiner les analyses.</t>
+  </si>
+  <si>
+    <t>Complexité du nettoyage des données et de leur mise en cohérence.
+|-|
+Importance d'une visualisation claire pour présenter efficacement les résultats et recommandations.</t>
+  </si>
+  <si>
+    <t>Identification des tendances tarifaires et des segments les plus compétitifs.
+|-|
+Recommandation claire d’une fourchette tarifaire optimale pour le Domaine des Croix.
+|-|
+Tableau de bord Power BI permettant une compréhension simple et intuitive du marché et des positionnements concurrentiels.</t>
+  </si>
+  <si>
+    <t>Python (Pandas, NumPy, Matplotlib, Seaborn, Skimpy, NLTK)
+|-|
+Power BI (visualisation interactive)
+|-|
+Jupyter Notebook
+|-|
+GitHub (gestion des versions)</t>
+  </si>
+  <si>
+    <t>Collecte et extraction des données.
+|-|
+Nettoyage et préparation des données avec Python (Pandas).
+|-|
+Analyse exploratoire approfondie (Pandas, Seaborn).
+|-|
+Comparaison spécifique du Pinot Noir bourguignon avec les vins similaires.
+|-|
+Élaboration de recommandations tarifaires par analyse statistique détaillée.
+|-|
+Création d’un tableau de bord interactif avec Power BI pour visualiser et communiquer les résultat</t>
+  </si>
+  <si>
+    <t>Analyser en profondeur le marché américain des vins, évaluer la position concurrentielle du vin du Domaine des Croix, et déterminer un prix ou une fourchette tarifaire optimale.</t>
+  </si>
+  <si>
+    <t>Besoin d'une analyse détaillée pour déterminer un positionnement tarifaire compétitif et valorisant sur un nouveau marché.</t>
+  </si>
+  <si>
+    <t>pwBI_data20_data.webp</t>
+  </si>
+  <si>
+    <t>Illustration des data skimpy</t>
+  </si>
+  <si>
+    <t>Ce projet de classification d'images a été réalisé dans le cadre d'une formation en Data Analyse avec une contrainte de temps de trente heures. L'objectif était d'entraîner un modèle de Deep Learning capable de classifier précisément différentes pièces de LEGO à partir d'images, afin de découvrir la computer vision.</t>
+  </si>
+  <si>
+    <t>Développer un modèle basé sur Keras capable de classifier correctement des photos de pièces de LEGO en différentes catégories distinctes.</t>
+  </si>
+  <si>
+    <t>5600 images au total réparties en 7 classes différentes (800 images par classe)</t>
+  </si>
+  <si>
+    <t>Données visuelles au format image (JPEG, PNG), et images 3D (.dae)</t>
+  </si>
+  <si>
+    <t>Un processus de Data Augmentation a été nécessaire en raison du nombre limité d'images initiales par classe</t>
+  </si>
+  <si>
+    <t>Augmenter la quantité et la diversité des données d'entraînement pour améliorer la précision du modèle.
+|-|
+Exploration de modèles de Deep Learning plus avancés ou de techniques d'ensemble pour une meilleure généralisation des prédictions.
+|-|
+Test de classification avec des images issues de contextes réels (angles variés, éclairages différents) pour valider la robustesse opérationnelle.</t>
+  </si>
+  <si>
+    <t>Gestion complexe du temps limité pour l’entraînement et l'optimisation du modèle.
+|-|
+Nécessité de maîtriser rapidement les techniques avancées de Deep Learning (Data Augmentation, optimisation des hyperparamètres).
+|-|
+Apprentissage pratique sur la manipulation et l'intégration de données visuelles et 3D dans un contexte de Deep Learning.</t>
+  </si>
+  <si>
+    <t>Un modèle capable de classifier efficacement des images LEGO en 7 catégories différentes avec une précision validée par une matrice de confusion claire.
+|-|
+Validation de la méthodologie de Data Augmentation pour renforcer les performances du modèle.</t>
+  </si>
+  <si>
+    <t>Python (Pandas, NumPy, Matplotlib, Pillow, seaborn, Scikit-learn)
+|-|
+TensorFlow et Keras pour l'entraînement du modèle
+|-|
+Jupyter Notebook et Google Colab</t>
+  </si>
+  <si>
+    <t>Collecte et organisation des données en catégories distinctes.
+|-|
+Prétraitement et augmentation des données pour améliorer les performances du modèle.
+|-|
+Construction et entraînement d'un modèle de Deep Learning en utilisant Keras et TensorFlow.
+|-|
+Évaluation du modèle à travers la précision (val_accuracy), la perte (val_loss) et une matrice de confusion.
+|-|
+Sauvegarde et test du modèle sur des données indépendantes.</t>
+  </si>
+  <si>
+    <t>Jeu de données collecté en ligne constitué d'images réelles et générées en 3D</t>
+  </si>
+  <si>
+    <t>image_class_data.webp</t>
+  </si>
+  <si>
+    <t>image_class_results.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">images d'une classe de lego plusieurs photos </t>
+  </si>
+  <si>
+    <t>Matrice de confusion sur le jeu de test</t>
+  </si>
+  <si>
+    <t>Projet développé durant une formation en Data Analyse visant à créer un système interactif et performant de recommandation de films basé sur la similitude et des caractéristiques extraites des bases de données IMDB et TMDB.</t>
+  </si>
+  <si>
+    <t>Développer un système de recommandation efficace utilisant des algorithmes de Machine Learning pour proposer des films adaptés, accompagné d'une visualisation claire et interactive des résultats.</t>
+  </si>
+  <si>
+    <t>Répondre à la difficulté des utilisateurs à choisir des films adaptés à leurs préférences et améliorer leur expérience utilisateur en proposant des recommandations.</t>
+  </si>
+  <si>
+    <t>Bases de données publiques IMDB et TMDB, API TMDB pour enrichir les données avec des images et informations complémentaires</t>
+  </si>
+  <si>
+    <t>Données vastes, issues de plusieurs milliers de films</t>
+  </si>
+  <si>
+    <t>Données quantitatives (notes, durées, années de sorties) et qualitatives (genres, acteurs, descriptions).</t>
+  </si>
+  <si>
+    <t>Données nécessitant un nettoyage approfondi et une harmonisation avant d’être utilisables pour le machine learning</t>
+  </si>
+  <si>
+    <t>Intégration d'algorithmes avancés de Machine learning pour améliorer la précision des recommandations en utilisant les descriptions de film.</t>
+  </si>
+  <si>
+    <t>Complexité de gestion des données hétérogènes provenant de différentes sources (IMDB et TMDB).
+|-|
+Importance cruciale du nettoyage et de la préparation des données avant l'entraînement du modèle.
+|-|
+Maîtrise des techniques de machine learning adaptées aux données catégorielles.</t>
+  </si>
+  <si>
+    <t>Un système interactif et efficace de recommandations de films personnalisé selon les goûts utilisateurs.
+|-|
+Visualisation claire des résultats et des principaux KPIs dans un application streamlit</t>
+  </si>
+  <si>
+    <t>Python (Pandas, NumPy, Matplotlib, Scikit-learn, Seaborn, Streamlit)
+|-|
+APIs IMDB et TMDB
+|-|
+Jupyter Notebook et Google Colab
+|-|
+GitHub pour le versionnement</t>
+  </si>
+  <si>
+    <t>Collecte et extraction des données IMDB et TMDB.
+|-|
+Nettoyage, jointures et exploration approfondie des données.
+|-|
+Identification des caractéristiques importantes pour le modèle.
+|-|
+Développement et entraînement d'un modèle de recommandation basé sur le machine learning.
+|-|
+Création d’une interface interactive avec Streamlit pour afficher les recommandations et les KPI associés.</t>
+  </si>
+  <si>
+    <t>flixoucreuse_results.webp</t>
+  </si>
+  <si>
+    <t>visualisation application streamlit</t>
+  </si>
+  <si>
+    <t>visualisation application streamlit page information</t>
+  </si>
+  <si>
+    <t>Ce projet vise à créer artificiellement des données représentatives d'une ligne de conditionnement automatisée. L'objectif est de permettre une visualisation réaliste des performances industrielles et d'analyser les paramètres influençant ces performances grâce à des données simulées précises.</t>
+  </si>
+  <si>
+    <t>Simuler précisément le comportement opérationnel d'une ligne automatisée pour étudier les cadences de production, l’impact des arrêts et les caractéristiques physiques des produits.</t>
+  </si>
+  <si>
+    <t>La nécessité de disposer de données détaillées pour analyser et optimiser les performances opérationnelles d'une ligne automatisée en conditions variées sans recourir à des données réelles.</t>
+  </si>
+  <si>
+    <t>Variable selon les paramètres de simulation, généralement étendue sur une période significative avec des intervalles d'une minute</t>
+  </si>
+  <si>
+    <t>Données générées artificiellement via des scripts Python</t>
+  </si>
+  <si>
+    <t>Données temporelles quantitatives et qualitatives représentant la cadence, les caractéristiques physiques (densité, viscosité), et les états opérationnels (production, arrêts programmés, arrêts non programmés).</t>
+  </si>
+  <si>
+    <t>Les données incluent des variations naturelles simulées comme la température extérieure et celle des produits, ainsi que des arrêts imprévus réalistes.</t>
+  </si>
+  <si>
+    <t>La gestion de la complexité des paramètres de simulation pour garantir un réalisme opérationnel.
+|-|
+Importance du calibrage précis des modèles de simulation pour obtenir des données réalistes surtout pour l'influence des températures extérieures.</t>
+  </si>
+  <si>
+    <t>Données simulées réalistes permettant une analyse approfondie des performances opérationnelles.
+|-|
+Identification claire des facteurs influençant la production grâce aux données simulées.</t>
+  </si>
+  <si>
+    <t>Python (Pandas, NumPy)
+|-|
+Scripts spécifiques pour simulation et génération de données
+|-|
+Outils d’analyse (Power BI, Jupyter Notebook)</t>
+  </si>
+  <si>
+    <t>Génération d'une liste de produits et leurs caractéristiques.
+|-|
+Simulation détaillée de la production incluant différentes phases opérationnelles.
+|-|
+Création d'une table de dates détaillée.
+|-|
+Simulation des conditions environnementales.
+|-|
+Génération finale des fichiers CSV exploitables pour l'analyse.</t>
+  </si>
+  <si>
+    <t>Ajout de différents scénarios de simulation pour étoffer les données générées.
+|-|
+Optimisation des scripts pour faciliter la personnalisation rapide des simulations.</t>
+  </si>
+  <si>
+    <t>Cette application répond à un besoin précis des clubs de judo de gérer efficacement les présences aux entraînements, d'offrir une gestion centralisée des cours et d'analyser statistiquement les fréquentations pour optimiser leur gestion.</t>
+  </si>
+  <si>
+    <t>Développer une application web intuitive permettant de suivre précisément les présences, gérer les informations des cours et des utilisateurs, et fournir des analyses statistiques utiles pour évaluer l'assiduité.</t>
+  </si>
+  <si>
+    <t>La nécessité d'améliorer la gestion administrative des clubs sportifs grâce à un outil numérique facilitant le suivi des judokas et l'analyse des fréquentations.</t>
+  </si>
+  <si>
+    <t>Données utilisateur collectées lors des présences aux entraînements, intégration avec France Judo pour les licenciers.</t>
+  </si>
+  <si>
+    <t>Données évolutives, variables selon le nombre d’utilisateurs et la fréquence des entraînements.</t>
+  </si>
+  <si>
+    <t>Données quantitatives (présences, statistiques fréquentations) et qualitatives (profils utilisateurs, catégories d'âge, cours).</t>
+  </si>
+  <si>
+    <t>Données sensibles nécessitant une gestion sécurisée et conforme à la réglementation sur la protection des données personnelles.</t>
+  </si>
+  <si>
+    <t>Ajout de fonctionnalités d’intelligence artificielle pour prédire les fréquentations via par exemple la saisonnalité.</t>
+  </si>
+  <si>
+    <t>Intégration sécurisée des données sensibles.
+|-|
+Nécessité de maîtriser plusieurs technologies (Flask, Docker, SQLAlchemy).</t>
+  </si>
+  <si>
+    <t>Application web opérationnelle simplifiant la gestion des présences et des cours.
+|-|
+Scrapping des informations licenciers via France Judo et connexion sécurisé de personnes ayant les droits d'extraire les informations.
+|-|
+Analyse statistique accessible améliorant la visibilité opérationnelle.
+|-|
+Lecture simplifiée des données de présence.</t>
+  </si>
+  <si>
+    <t>Backend : Python (Flask, SQLAlchemy)
+|-|
+Frontend : HTML, CSS, JavaScript (Swiper.js)
+|-|
+Base de données : MySQL
+|-|
+Docker pour la conteneurisation
+|-|
+GitHub pour le versionnement</t>
+  </si>
+  <si>
+    <t>Développement du backend avec Flask et SQLAlchemy.
+|-|
+Création de la base de données MySQL et structuration des données.
+Développement d’une interface utilisateur conviviale en HTML, CSS et JavaScript.
+|-|
+Mise en place de l’authentification sécurisée.
+|-|
+Intégration des fonctionnalités statistiques.
+|-|
+Conteneurisation de l’application avec Docker.
+|-|
+Déploiement de l’application.</t>
+  </si>
+  <si>
+    <t>Ce projet industriel est centré sur l'analyse détaillée des performances d'une ligne de conditionnement automatisée. L'objectif est de déterminer précisément quels facteurs (densité, viscosité, caractéristiques physiques des produits, conditions environnementales et types d'emballage) influencent significativement la performance opérationnelle, afin de proposer des leviers d'amélioration concrets.</t>
+  </si>
+  <si>
+    <t>Identifier clairement les paramètres critiques qui affectent la cadence et la performance globale d'une ligne de conditionnement afin d'en améliorer l'efficacité opérationnelle</t>
+  </si>
+  <si>
+    <t>Comment optimiser la performance d'une ligne de conditionnement en identifiant et en contrôlant les principaux facteurs d'influence sur la cadence et la fiabilité opérationnelle ?</t>
+  </si>
+  <si>
+    <t>Développement d'un modèle prédictif pour anticiper les impacts des variations de paramètres en temps réel.
+|-|
+Intégration de scénarios plus diversifiés pour mieux anticiper les performances sous différentes conditions opérationnelles.</t>
+  </si>
+  <si>
+    <t>Identification des principaux paramètres impactant la performance (densité, viscosité, ratio produit/cadence).
+|-|
+Proposition de recommandations pratiques pour optimiser la cadence.</t>
+  </si>
+  <si>
+    <t>Les données intègrent des anomalies et des irrégularités temporelles.</t>
+  </si>
+  <si>
+    <t>Extraction et consolidation des données depuis la base SQL Server.
+|-|
+Nettoyage et prétraitement des données temporelles avec Python.
+|-|
+Développement des mesures analytiques en DAX.
+|-|
+Création du rapport interactif avec Power BI.
+|-|
+Mise en place de mesures d'amélioration</t>
+  </si>
+  <si>
+    <t>Extraction et consolidation des données depuis la base de données.
+|-|
+Nettoyage et prétraitement des données temporelles.
+|-|
+Développement des mesures analytiques en DAX.
+|-|
+Création du rapport interactif avec Power BI.
+|-|
+Mise en place de mesures d'amélioration</t>
+  </si>
+  <si>
+    <t>facteurs_influence_results.webp</t>
+  </si>
+  <si>
+    <t>facteurs_influence_data.webp</t>
+  </si>
+  <si>
+    <t>flixoucreuse_data.webp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,6 +820,14 @@
       <sz val="11"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -364,28 +873,146 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="28">
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -396,6 +1023,41 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA343F91-ABD2-41F5-B074-A3DB5ED79D55}" name="Tableau1" displayName="Tableau1" ref="A1:Z10" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A1:Z10" xr:uid="{BA343F91-ABD2-41F5-B074-A3DB5ED79D55}"/>
+  <tableColumns count="26">
+    <tableColumn id="1" xr3:uid="{7E76F91B-E618-41EE-9C37-B7202AB690DD}" name="id" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{4A6F015C-59BD-48A4-9884-9E28BA1294A4}" name="title" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{01EB81F2-B04C-43B2-8D3B-3DAA19ECF415}" name="description" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{6534B8D9-E907-4BC2-8788-A60BF8C38512}" name="image_url" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{8F826BC0-97B6-48DC-B535-ADEE2F1B649E}" name="image_alt" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{574F570A-18F3-4000-BDE3-83B7EE7A33BE}" name="tags" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{699FA15F-FD6A-4B94-9225-CAAD7C6545DA}" name="description_detail" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{6BC2C552-52A7-439D-843A-68F3486D8D87}" name="objectif_projet" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{EC928EC9-7B64-496B-AF1F-E45343203EF7}" name="Probleme_resolu" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{9104D129-D3BA-4E5E-BA1E-BC76245DBC60}" name="data_source" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{8C6A8EDC-0C5F-441D-898F-EEBDF9CC02E0}" name="data_size" dataDxfId="15"/>
+    <tableColumn id="12" xr3:uid="{DB23C4AA-C25C-4F2C-BDF4-AED3372333E3}" name="data_type" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{E0842EEC-4206-4C08-91FF-7F7760EE4E81}" name="data_remark" dataDxfId="13"/>
+    <tableColumn id="14" xr3:uid="{5C91EE04-3E23-4E51-AF03-7150476816C1}" name="url_img_data" dataDxfId="12"/>
+    <tableColumn id="15" xr3:uid="{ABDDD609-BAE0-40F8-8802-E54082C0A6FA}" name="alt_img_data" dataDxfId="11"/>
+    <tableColumn id="16" xr3:uid="{4ADFAE86-3986-4940-B453-C946FFD7C9E6}" name="project_steps" dataDxfId="10"/>
+    <tableColumn id="17" xr3:uid="{49A4ADD7-02AF-4B22-B891-A75758FB681A}" name="techno" dataDxfId="9"/>
+    <tableColumn id="18" xr3:uid="{C1626FB7-43B5-48C6-94EC-6B0B88154189}" name="result" dataDxfId="8"/>
+    <tableColumn id="19" xr3:uid="{8012E277-42C6-4B8E-BE6E-679FCD796CBB}" name="img_results" dataDxfId="7"/>
+    <tableColumn id="20" xr3:uid="{23DCDF7C-22E8-49B4-A027-B8FA550C2CC8}" name="alt_img_results" dataDxfId="6"/>
+    <tableColumn id="21" xr3:uid="{AAD7C8DA-C396-4440-ABD3-1C9F99A9F70A}" name="powerbi_link" dataDxfId="5"/>
+    <tableColumn id="22" xr3:uid="{01CC34CC-A477-4637-AAEB-EA8D3B91B7B2}" name="github_link" dataDxfId="4"/>
+    <tableColumn id="23" xr3:uid="{BF856CDB-8E06-4FEF-98B3-A6B13477DC33}" name="streamlit_link" dataDxfId="3"/>
+    <tableColumn id="24" xr3:uid="{DA2CC5FB-F5D0-4B62-B17D-44C236CCCD8D}" name="video_link" dataDxfId="2"/>
+    <tableColumn id="25" xr3:uid="{B40FC4B2-4C85-474B-84F2-CCB290ABA8C2}" name="difficulties_learns" dataDxfId="1"/>
+    <tableColumn id="26" xr3:uid="{7BD0E41A-775D-478B-97C4-8EED85D35711}" name="potential_improvement" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -685,387 +1347,789 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="M8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="121.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="58.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="104" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="17.7109375" customWidth="1"/>
-    <col min="16" max="16" width="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="24.28515625" customWidth="1"/>
-    <col min="21" max="21" width="165.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="47.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="32.7109375" customWidth="1"/>
-    <col min="25" max="25" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="68.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="6" max="6" width="55.7109375" customWidth="1"/>
+    <col min="7" max="7" width="82.85546875" customWidth="1"/>
+    <col min="8" max="8" width="48" customWidth="1"/>
+    <col min="9" max="9" width="40.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="23" customWidth="1"/>
+    <col min="12" max="12" width="21" customWidth="1"/>
+    <col min="13" max="13" width="29.85546875" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" customWidth="1"/>
+    <col min="15" max="15" width="26.140625" customWidth="1"/>
+    <col min="16" max="16" width="28.140625" customWidth="1"/>
+    <col min="17" max="17" width="44.7109375" customWidth="1"/>
+    <col min="18" max="18" width="97.5703125" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.140625" customWidth="1"/>
+    <col min="21" max="21" width="35.140625" customWidth="1"/>
+    <col min="22" max="22" width="20" customWidth="1"/>
+    <col min="23" max="24" width="17.5703125" customWidth="1"/>
+    <col min="25" max="26" width="66.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:26" ht="240" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="U2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="U2" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:26" ht="225" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="U3" t="s">
+      <c r="G3" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2" t="s">
+        <v>194</v>
+      </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:26" ht="270" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="U4" t="s">
+      <c r="G4" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="U4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V4" t="s">
+      <c r="V4" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>116</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:26" ht="360" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="U5" t="s">
+      <c r="G5" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="U5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="V5" t="s">
+      <c r="V5" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="6" spans="1:26" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:26" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="N6" t="s">
+      <c r="M6" s="2"/>
+      <c r="N6" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="R6" s="3" t="s">
+      <c r="R6" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="S6" t="s">
+      <c r="S6" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="T6" t="s">
+      <c r="T6" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="V6" t="s">
+      <c r="U6" s="2"/>
+      <c r="V6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="X6" t="s">
+      <c r="W6" s="2"/>
+      <c r="X6" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="Y6" s="3" t="s">
+      <c r="Y6" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="Z6" s="3" t="s">
+      <c r="Z6" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:26" ht="345" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="V7" t="s">
+      <c r="G7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z7" s="2" t="s">
+        <v>142</v>
+      </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:26" ht="315" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="V8" t="s">
+      <c r="G8" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="W8" t="s">
+      <c r="W8" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="Z8" s="2" t="s">
+        <v>159</v>
+      </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:26" ht="270" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="V9" t="s">
+      <c r="G9" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="Z9" s="2" t="s">
+        <v>178</v>
+      </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:26" ht="315" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="V10" t="s">
+      <c r="G10" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="Z10" s="2" t="s">
+        <v>186</v>
+      </c>
     </row>
+    <row r="11" spans="1:26" ht="85.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:26" ht="85.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q23" s="4"/>
+      <c r="Q23" s="1"/>
     </row>
     <row r="24" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q24" s="4"/>
+      <c r="Q24" s="1"/>
     </row>
     <row r="25" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q25" s="4"/>
+      <c r="Q25" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="U2" r:id="rId1" xr:uid="{4932D6DB-80F0-44AA-8099-9A1E7EAE4CF4}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>